<commit_message>
Introduction updates, new articles
</commit_message>
<xml_diff>
--- a/01_Thesis/Articles/MSc_article matrix.xlsx
+++ b/01_Thesis/Articles/MSc_article matrix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\00_ERAN\Academics\MSc\msc_repo_2\01_Thesis\Articles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A81F5B6-E30E-4859-BD44-9C58D3AADC77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04515C7E-D233-48E9-8AE8-DE2815306E1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>Article name</t>
   </si>
@@ -145,6 +145,12 @@
   </si>
   <si>
     <t>Glykys et al.</t>
+  </si>
+  <si>
+    <t>THE COMPOSITION OF ANIMAL CELLS: SOLUTES CONTRIBUTING TO OSMOTIC PRESSURE AND CHARGE BALANCE</t>
+  </si>
+  <si>
+    <t>Burton</t>
   </si>
 </sst>
 </file>
@@ -502,7 +508,7 @@
   <dimension ref="A2:L33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -832,82 +838,98 @@
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>14</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B17" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" t="s">
+        <v>41</v>
+      </c>
+      <c r="D17">
+        <v>1983</v>
+      </c>
+      <c r="E17" s="2"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>27</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>29</v>
       </c>

</xml_diff>